<commit_message>
version beta todo funciona
</commit_message>
<xml_diff>
--- a/web/Excel/GIL-F-014_Formato_Solicitud_de_Bienes.xlsx
+++ b/web/Excel/GIL-F-014_Formato_Solicitud_de_Bienes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t xml:space="preserve">SERVICIO NACIONAL DE APRENDIZAJE SENA </t>
   </si>
@@ -37,31 +37,31 @@
     <t>CUENTADANTES QUE  TIENEN VINCULO CON LA ENTIDAD</t>
   </si>
   <si>
-    <t>FECHA SOLICITUD:  2021-07-15</t>
-  </si>
-  <si>
-    <t>AREA: ghgh</t>
-  </si>
-  <si>
-    <t>NOMBRE CENTRO DE COSTO: cdti</t>
+    <t>FECHA SOLICITUD:  2021-07-02</t>
+  </si>
+  <si>
+    <t>AREA: Compras</t>
+  </si>
+  <si>
+    <t>NOMBRE CENTRO DE COSTO: Centro de Diseño tecnologico industrial</t>
   </si>
   <si>
     <t>NOMBRE REGIONAL:  regional valle</t>
   </si>
   <si>
-    <t>NOMBRE DE JEFE DE OFICINA O COORDINADOR DE AREA: vggcg</t>
-  </si>
-  <si>
-    <t>CEDULA: 567654</t>
-  </si>
-  <si>
-    <t>NOMBRE DE SERVIDOR PÚBLICO A QUIEN SE LE ASIGNARA EL BIEN: vggcg</t>
-  </si>
-  <si>
-    <t>CEDULA: 87756</t>
-  </si>
-  <si>
-    <t>CÓDIGO DE GRUPO O FICHA DE CARACTERIZACIÓN: 2346</t>
+    <t>NOMBRE DE JEFE DE OFICINA O COORDINADOR DE AREA: jair</t>
+  </si>
+  <si>
+    <t>CEDULA: 11111111</t>
+  </si>
+  <si>
+    <t>NOMBRE DE SERVIDOR PÚBLICO A QUIEN SE LE ASIGNARA EL BIEN: jair</t>
+  </si>
+  <si>
+    <t>CEDULA: 1111111</t>
+  </si>
+  <si>
+    <t>CÓDIGO DE GRUPO O FICHA DE CARACTERIZACIÓN: 123456</t>
   </si>
   <si>
     <t>ITEM</t>
@@ -79,10 +79,13 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>Papelillo</t>
-  </si>
-  <si>
-    <t>Cg- centrigramo</t>
+    <t>Reprograf</t>
+  </si>
+  <si>
+    <t>Cm - Centimetro</t>
+  </si>
+  <si>
+    <t>n/aa</t>
   </si>
   <si>
     <t xml:space="preserve">NOMBRE: </t>
@@ -839,26 +842,26 @@
         <v>21</v>
       </c>
       <c r="E21" s="14">
-        <v>5656</v>
-      </c>
-      <c r="F21" s="14">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="B32" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="4"/>
       <c r="E32" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6">
       <c r="B33" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="4"/>

</xml_diff>